<commit_message>
Working On Data flow
</commit_message>
<xml_diff>
--- a/ProductManagement.xlsx
+++ b/ProductManagement.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chip1stop-my.sharepoint.com/personal/aoza_chip1stop_com/Documents/デスクトップ/projectmanagement/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABHISHEK\Desktop\management\Project_Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{6145F318-18BF-4D67-A638-F43F0A70F1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C86D4F6C-8484-4A71-91B3-42CA131058EE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66018C1D-9AB0-40DB-BC90-685594375116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{4339B1FC-E328-4227-9E41-8F7320B7A6CB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4339B1FC-E328-4227-9E41-8F7320B7A6CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,23 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>Root Layout</t>
     <phoneticPr fontId="1"/>
@@ -216,6 +205,36 @@
   <si>
     <t>dataTable</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sample Data  In Projects</t>
+  </si>
+  <si>
+    <t>Date Required for Charts'</t>
+  </si>
+  <si>
+    <t>1. create api for avaliable vendors</t>
+  </si>
+  <si>
+    <t>/vendors/available</t>
+  </si>
+  <si>
+    <t>2.select the vendor  from the dropdown</t>
+  </si>
+  <si>
+    <t>3.Bill should have link and not displayed on card</t>
+  </si>
+  <si>
+    <t>4.task status /optional</t>
+  </si>
+  <si>
+    <t>Sample Data requirements in Client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client will have data and column and then button to edit and its info and delete it </t>
+  </si>
+  <si>
+    <t xml:space="preserve">when client info is stored while registering a project </t>
   </si>
 </sst>
 </file>
@@ -226,14 +245,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -242,7 +261,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="游ゴシック"/>
+      <name val="Aptos Narrow"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -282,7 +301,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1833,6 +1852,178 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>605790</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="正方形/長方形 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB5F4099-3EA0-41A7-A626-B8DABA539C2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1882140" y="14058900"/>
+          <a:ext cx="2381250" cy="2007870"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>2540</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="直線コネクタ 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DC18E9A-1D7C-4542-8995-EDC3686AFDA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2438400" y="14081760"/>
+          <a:ext cx="6350" cy="2014220"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="正方形/長方形 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B94A5D3B-2E02-4DA3-B283-DCD033455FC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2529840" y="14165580"/>
+          <a:ext cx="647700" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2559,13 +2750,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467E8FF1-2935-4268-8D94-68117082996D}">
   <dimension ref="D3:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="J72" sqref="J72"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="G93" sqref="F87:G93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>0</v>
       </c>
@@ -2581,7 +2772,7 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="4:18" x14ac:dyDescent="0.2">
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -2589,7 +2780,7 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="7" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="4:18" x14ac:dyDescent="0.2">
       <c r="N7" s="2" t="s">
         <v>13</v>
       </c>
@@ -2598,31 +2789,31 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="4:18" x14ac:dyDescent="0.2">
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="4:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="4:18" x14ac:dyDescent="0.2">
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="4:15" x14ac:dyDescent="0.2">
       <c r="L19" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>0</v>
       </c>
@@ -2630,17 +2821,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="4:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="4:15" x14ac:dyDescent="0.2">
       <c r="O21" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="4:15" x14ac:dyDescent="0.2">
       <c r="N28" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="4:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D35" t="s">
         <v>5</v>
       </c>
@@ -2648,7 +2839,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="4:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D36" t="s">
         <v>8</v>
       </c>
@@ -2656,17 +2847,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="4:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="4:14" x14ac:dyDescent="0.2">
       <c r="N37" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="4:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="4:14" x14ac:dyDescent="0.2">
       <c r="N40" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="4:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D52" t="s">
         <v>26</v>
       </c>
@@ -2674,12 +2865,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="4:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="4:14" x14ac:dyDescent="0.2">
       <c r="I55" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="4:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="4:14" x14ac:dyDescent="0.2">
       <c r="I56" t="s">
         <v>28</v>
       </c>
@@ -2687,12 +2878,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="4:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="4:14" x14ac:dyDescent="0.2">
       <c r="I57" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="4:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="4:14" x14ac:dyDescent="0.2">
       <c r="I59" t="s">
         <v>30</v>
       </c>
@@ -2700,17 +2891,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="4:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="4:14" x14ac:dyDescent="0.2">
       <c r="I60" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="4:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="4:14" x14ac:dyDescent="0.2">
       <c r="I62" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="4:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="4:14" x14ac:dyDescent="0.2">
       <c r="I63" t="s">
         <v>33</v>
       </c>
@@ -2731,12 +2922,12 @@
   <dimension ref="B2:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>14</v>
       </c>
@@ -2744,7 +2935,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -2752,7 +2943,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -2763,12 +2954,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -2788,9 +2979,9 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>17</v>
       </c>
@@ -2798,12 +2989,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I10" t="s">
         <v>21</v>
       </c>
@@ -2817,37 +3008,77 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E4C59B-3CED-4FE1-8ECA-90FF143BC51E}">
-  <dimension ref="C5:C10"/>
+  <dimension ref="C5:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="I6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="I7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="I9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>41</v>
+      </c>
+      <c r="I10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="I16" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2864,14 +3095,14 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Vendor List segregation inProcess
</commit_message>
<xml_diff>
--- a/ProductManagement.xlsx
+++ b/ProductManagement.xlsx
@@ -5,19 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABHISHEK\Desktop\management\Project_Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project_Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66018C1D-9AB0-40DB-BC90-685594375116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC23F25-34B0-4EA6-8EB3-3AC4B2A8E990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4339B1FC-E328-4227-9E41-8F7320B7A6CB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{4339B1FC-E328-4227-9E41-8F7320B7A6CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Shadcnui" sheetId="3" r:id="rId2"/>
-    <sheet name="DataDisplay" sheetId="2" r:id="rId3"/>
-    <sheet name="apis" sheetId="4" r:id="rId4"/>
-    <sheet name="components" sheetId="5" r:id="rId5"/>
+    <sheet name="Packages to delete after test" sheetId="6" r:id="rId2"/>
+    <sheet name="Shadcnui" sheetId="3" r:id="rId3"/>
+    <sheet name="DataDisplay" sheetId="2" r:id="rId4"/>
+    <sheet name="apis" sheetId="4" r:id="rId5"/>
+    <sheet name="components" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>Root Layout</t>
     <phoneticPr fontId="1"/>
@@ -235,6 +236,10 @@
   </si>
   <si>
     <t xml:space="preserve">when client info is stored while registering a project </t>
+  </si>
+  <si>
+    <t>uuid</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -245,14 +250,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Aptos Narrow"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -261,7 +266,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
+      <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -301,7 +306,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2750,13 +2755,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467E8FF1-2935-4268-8D94-68117082996D}">
   <dimension ref="D3:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="G93" sqref="F87:G93"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="N67" sqref="N67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="3" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="4:18" x14ac:dyDescent="0.55000000000000004">
       <c r="D3" t="s">
         <v>0</v>
       </c>
@@ -2772,7 +2777,7 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="4:18" x14ac:dyDescent="0.55000000000000004">
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -2780,7 +2785,7 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="7" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="4:18" x14ac:dyDescent="0.55000000000000004">
       <c r="N7" s="2" t="s">
         <v>13</v>
       </c>
@@ -2789,31 +2794,31 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="4:18" x14ac:dyDescent="0.55000000000000004">
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="4:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="4:18" x14ac:dyDescent="0.55000000000000004">
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:15" x14ac:dyDescent="0.55000000000000004">
       <c r="D18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:15" x14ac:dyDescent="0.55000000000000004">
       <c r="L19" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:15" x14ac:dyDescent="0.55000000000000004">
       <c r="D20" t="s">
         <v>0</v>
       </c>
@@ -2821,17 +2826,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:15" x14ac:dyDescent="0.55000000000000004">
       <c r="O21" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:15" x14ac:dyDescent="0.55000000000000004">
       <c r="N28" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D35" t="s">
         <v>5</v>
       </c>
@@ -2839,7 +2844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D36" t="s">
         <v>8</v>
       </c>
@@ -2847,17 +2852,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="N37" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="N40" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D52" t="s">
         <v>26</v>
       </c>
@@ -2865,12 +2870,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="I55" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="I56" t="s">
         <v>28</v>
       </c>
@@ -2878,12 +2883,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="I57" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="I59" t="s">
         <v>30</v>
       </c>
@@ -2891,17 +2896,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="I60" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="I62" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="4:14" x14ac:dyDescent="0.55000000000000004">
       <c r="I63" t="s">
         <v>33</v>
       </c>
@@ -2918,6 +2923,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA085582-6A0A-4026-ABDF-ED128CBA4FFF}">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04CBCF92-9814-4C9A-8333-1EFFA168AD92}">
   <dimension ref="B2:H6"/>
   <sheetViews>
@@ -2925,9 +2951,9 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
         <v>14</v>
       </c>
@@ -2935,7 +2961,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -2943,7 +2969,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -2954,49 +2980,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
         <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE4831F-1065-46C4-974E-48B604B01A4F}">
-  <dimension ref="B3:I10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="I6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="I10" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -3007,6 +2998,41 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE4831F-1065-46C4-974E-48B604B01A4F}">
+  <dimension ref="B3:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E4C59B-3CED-4FE1-8ECA-90FF143BC51E}">
   <dimension ref="C5:Q16"/>
   <sheetViews>
@@ -3014,9 +3040,9 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="5" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" t="s">
         <v>37</v>
       </c>
@@ -3024,7 +3050,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" t="s">
         <v>38</v>
       </c>
@@ -3032,7 +3058,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" t="s">
         <v>39</v>
       </c>
@@ -3040,12 +3066,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="I8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" t="s">
         <v>40</v>
       </c>
@@ -3053,7 +3079,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="C10" t="s">
         <v>41</v>
       </c>
@@ -3061,22 +3087,22 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="C12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="I14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="I15" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="I16" t="s">
         <v>53</v>
       </c>
@@ -3087,7 +3113,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE7240E6-B94E-4220-8DDD-D30F02E0F421}">
   <dimension ref="C4:C5"/>
   <sheetViews>
@@ -3095,14 +3121,14 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
tasks input in progress
</commit_message>
<xml_diff>
--- a/ProductManagement.xlsx
+++ b/ProductManagement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project_Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC23F25-34B0-4EA6-8EB3-3AC4B2A8E990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC9DD0D-1BE5-418E-A457-FD833A2E26BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{4339B1FC-E328-4227-9E41-8F7320B7A6CB}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="8260" activeTab="1" xr2:uid="{4339B1FC-E328-4227-9E41-8F7320B7A6CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
   <si>
     <t>Root Layout</t>
     <phoneticPr fontId="1"/>
@@ -239,6 +239,14 @@
   </si>
   <si>
     <t>uuid</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">handle text-alignment </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>project id is number other all ids are string so handle that</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2755,7 +2763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467E8FF1-2935-4268-8D94-68117082996D}">
   <dimension ref="D3:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+    <sheetView topLeftCell="A97" workbookViewId="0">
       <selection activeCell="N67" sqref="N67"/>
     </sheetView>
   </sheetViews>
@@ -2924,10 +2932,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA085582-6A0A-4026-ABDF-ED128CBA4FFF}">
-  <dimension ref="B2"/>
+  <dimension ref="B2:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -2935,6 +2943,16 @@
     <row r="2" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Toast hook created/ working on nodemailer
</commit_message>
<xml_diff>
--- a/ProductManagement.xlsx
+++ b/ProductManagement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project_Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC9DD0D-1BE5-418E-A457-FD833A2E26BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E1C632-2C51-4B6E-B460-3EB9C306F58A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="8260" activeTab="1" xr2:uid="{4339B1FC-E328-4227-9E41-8F7320B7A6CB}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="8260" activeTab="1" xr2:uid="{4339B1FC-E328-4227-9E41-8F7320B7A6CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>Root Layout</t>
     <phoneticPr fontId="1"/>
@@ -247,6 +247,18 @@
   </si>
   <si>
     <t>project id is number other all ids are string so handle that</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>toast---&gt; add</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>api fetching plus for whom to use Memo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>user schema development</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2932,10 +2944,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA085582-6A0A-4026-ABDF-ED128CBA4FFF}">
-  <dimension ref="B2:B4"/>
+  <dimension ref="B2:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -2953,6 +2965,21 @@
     <row r="4" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>